<commit_message>
Update to budget calculations Excel
</commit_message>
<xml_diff>
--- a/Notes/budget_calculations.xlsx
+++ b/Notes/budget_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0721CA9-E968-4CEE-B881-9D68B73C7110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8AED94-8E36-4B3C-9D0F-8D16DB6293D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{60A3E455-5768-4DE3-BCE2-5116B63F6CFB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60A3E455-5768-4DE3-BCE2-5116B63F6CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="linear_increases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>time steps</t>
   </si>
@@ -72,6 +72,21 @@
   </si>
   <si>
     <t>with the linear decreases, I do not need a formula to calculate the incremenets because the 10,000 limit is an upper limit, not a lower limit</t>
+  </si>
+  <si>
+    <t>The equation still holds and produces 1275</t>
+  </si>
+  <si>
+    <t>If I want the budget to start from 100 (rather than 0) but still add up to 10,000</t>
+  </si>
+  <si>
+    <t>5000 = x + 2x + 3x…50x</t>
+  </si>
+  <si>
+    <t>But now it is 5000 = 1275x</t>
+  </si>
+  <si>
+    <t>Therefore x = 5000/1275</t>
   </si>
 </sst>
 </file>
@@ -755,6 +770,407 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>linear_increases!$C$6:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207.84313725490196</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>215.68627450980392</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>223.52941176470588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>231.37254901960785</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>239.21568627450981</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>247.05882352941177</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>254.90196078431373</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>262.74509803921569</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270.58823529411762</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>278.43137254901956</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>286.27450980392149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>294.11764705882342</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>301.96078431372536</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>309.80392156862729</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>317.64705882352922</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>325.49019607843115</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>333.33333333333309</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>341.17647058823502</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>349.01960784313695</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>356.86274509803889</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>364.70588235294082</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>372.54901960784275</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>380.39215686274468</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>388.23529411764662</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>396.07843137254855</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>403.92156862745048</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>411.76470588235242</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>419.60784313725435</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>427.45098039215628</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>435.29411764705821</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>443.13725490196015</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>450.98039215686208</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>458.82352941176401</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>466.66666666666595</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>474.50980392156788</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>482.35294117646981</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>490.19607843137175</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>498.03921568627368</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>505.88235294117561</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>513.72549019607754</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>521.56862745097953</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>529.41176470588152</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>537.25490196078351</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>545.0980392156855</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>552.94117647058749</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>560.78431372548948</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>568.62745098039147</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>576.47058823529346</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>584.31372549019545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0D1-424A-9D4B-3136E3EFD8A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1622923264"/>
+        <c:axId val="1622923680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1622923264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1622923680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1622923680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1622923264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1392,6 +1808,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2424,20 +2880,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>62865</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>62865</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>177165</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2457,6 +3429,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B5638E-735C-42AE-BEDB-E03AB77C622A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3221,8 +4229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070648CE-F5EC-498A-AC01-A907055F7282}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3276,6 +4284,12 @@
         <f>A6*$F$6</f>
         <v>7.8431372549019605</v>
       </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
       <c r="F6">
         <f>10000/1275</f>
         <v>7.8431372549019605</v>
@@ -3289,6 +4303,14 @@
         <f t="shared" ref="B7:B55" si="0">A7*$F$6</f>
         <v>15.686274509803921</v>
       </c>
+      <c r="C7">
+        <f>C6+$B$6</f>
+        <v>207.84313725490196</v>
+      </c>
+      <c r="D7">
+        <f>D6+$F$14</f>
+        <v>103.92156862745098</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3298,6 +4320,14 @@
         <f t="shared" si="0"/>
         <v>23.52941176470588</v>
       </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C55" si="1">C7+$B$6</f>
+        <v>215.68627450980392</v>
+      </c>
+      <c r="D8">
+        <f>D7+$F$14</f>
+        <v>107.84313725490196</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -3307,6 +4337,17 @@
         <f t="shared" si="0"/>
         <v>31.372549019607842</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>223.52941176470588</v>
+      </c>
+      <c r="D9">
+        <f>D8+$F$14</f>
+        <v>111.76470588235294</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -3316,6 +4357,17 @@
         <f t="shared" si="0"/>
         <v>39.2156862745098</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>231.37254901960785</v>
+      </c>
+      <c r="D10">
+        <f>D9+$F$14</f>
+        <v>115.68627450980392</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -3325,6 +4377,17 @@
         <f t="shared" si="0"/>
         <v>47.058823529411761</v>
       </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>239.21568627450981</v>
+      </c>
+      <c r="D11">
+        <f>D10+$F$14</f>
+        <v>119.6078431372549</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -3334,6 +4397,17 @@
         <f t="shared" si="0"/>
         <v>54.901960784313722</v>
       </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>247.05882352941177</v>
+      </c>
+      <c r="D12">
+        <f>D11+$F$14</f>
+        <v>123.52941176470588</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3343,6 +4417,17 @@
         <f t="shared" si="0"/>
         <v>62.745098039215684</v>
       </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>254.90196078431373</v>
+      </c>
+      <c r="D13">
+        <f>D12+$F$14</f>
+        <v>127.45098039215686</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3352,6 +4437,18 @@
         <f t="shared" si="0"/>
         <v>70.588235294117638</v>
       </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>262.74509803921569</v>
+      </c>
+      <c r="D14">
+        <f>D13+$F$14</f>
+        <v>131.37254901960785</v>
+      </c>
+      <c r="F14">
+        <f>5000/1275</f>
+        <v>3.9215686274509802</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -3361,6 +4458,14 @@
         <f t="shared" si="0"/>
         <v>78.431372549019599</v>
       </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>270.58823529411762</v>
+      </c>
+      <c r="D15">
+        <f>D14+$F$14</f>
+        <v>135.29411764705881</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3370,8 +4475,16 @@
         <f t="shared" si="0"/>
         <v>86.274509803921561</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>278.43137254901956</v>
+      </c>
+      <c r="D16">
+        <f>D15+$F$14</f>
+        <v>139.21568627450978</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -3379,8 +4492,16 @@
         <f t="shared" si="0"/>
         <v>94.117647058823522</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>286.27450980392149</v>
+      </c>
+      <c r="D17">
+        <f>D16+$F$14</f>
+        <v>143.13725490196074</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -3388,8 +4509,16 @@
         <f t="shared" si="0"/>
         <v>101.96078431372548</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>294.11764705882342</v>
+      </c>
+      <c r="D18">
+        <f>D17+$F$14</f>
+        <v>147.05882352941171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>14</v>
       </c>
@@ -3397,8 +4526,16 @@
         <f t="shared" si="0"/>
         <v>109.80392156862744</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>301.96078431372536</v>
+      </c>
+      <c r="D19">
+        <f>D18+$F$14</f>
+        <v>150.98039215686268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15</v>
       </c>
@@ -3406,8 +4543,16 @@
         <f t="shared" si="0"/>
         <v>117.64705882352941</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>309.80392156862729</v>
+      </c>
+      <c r="D20">
+        <f>D19+$F$14</f>
+        <v>154.90196078431364</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -3415,8 +4560,16 @@
         <f t="shared" si="0"/>
         <v>125.49019607843137</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>317.64705882352922</v>
+      </c>
+      <c r="D21">
+        <f>D20+$F$14</f>
+        <v>158.82352941176461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
@@ -3424,8 +4577,16 @@
         <f t="shared" si="0"/>
         <v>133.33333333333331</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>325.49019607843115</v>
+      </c>
+      <c r="D22">
+        <f>D21+$F$14</f>
+        <v>162.74509803921558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -3433,8 +4594,16 @@
         <f t="shared" si="0"/>
         <v>141.17647058823528</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>333.33333333333309</v>
+      </c>
+      <c r="D23">
+        <f>D22+$F$14</f>
+        <v>166.66666666666654</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -3442,8 +4611,16 @@
         <f t="shared" si="0"/>
         <v>149.01960784313724</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>341.17647058823502</v>
+      </c>
+      <c r="D24">
+        <f>D23+$F$14</f>
+        <v>170.58823529411751</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
@@ -3451,8 +4628,16 @@
         <f t="shared" si="0"/>
         <v>156.8627450980392</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>349.01960784313695</v>
+      </c>
+      <c r="D25">
+        <f>D24+$F$14</f>
+        <v>174.50980392156848</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -3460,8 +4645,16 @@
         <f t="shared" si="0"/>
         <v>164.70588235294116</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>356.86274509803889</v>
+      </c>
+      <c r="D26">
+        <f>D25+$F$14</f>
+        <v>178.43137254901944</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -3469,8 +4662,16 @@
         <f t="shared" si="0"/>
         <v>172.54901960784312</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>364.70588235294082</v>
+      </c>
+      <c r="D27">
+        <f>D26+$F$14</f>
+        <v>182.35294117647041</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>23</v>
       </c>
@@ -3478,8 +4679,16 @@
         <f t="shared" si="0"/>
         <v>180.39215686274508</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>372.54901960784275</v>
+      </c>
+      <c r="D28">
+        <f>D27+$F$14</f>
+        <v>186.27450980392138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>24</v>
       </c>
@@ -3487,8 +4696,16 @@
         <f t="shared" si="0"/>
         <v>188.23529411764704</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>380.39215686274468</v>
+      </c>
+      <c r="D29">
+        <f>D28+$F$14</f>
+        <v>190.19607843137234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>25</v>
       </c>
@@ -3496,8 +4713,16 @@
         <f t="shared" si="0"/>
         <v>196.07843137254901</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>388.23529411764662</v>
+      </c>
+      <c r="D30">
+        <f>D29+$F$14</f>
+        <v>194.11764705882331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>26</v>
       </c>
@@ -3505,8 +4730,16 @@
         <f t="shared" si="0"/>
         <v>203.92156862745097</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>396.07843137254855</v>
+      </c>
+      <c r="D31">
+        <f>D30+$F$14</f>
+        <v>198.03921568627428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>27</v>
       </c>
@@ -3514,8 +4747,16 @@
         <f t="shared" si="0"/>
         <v>211.76470588235293</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>403.92156862745048</v>
+      </c>
+      <c r="D32">
+        <f>D31+$F$14</f>
+        <v>201.96078431372524</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>28</v>
       </c>
@@ -3523,8 +4764,16 @@
         <f t="shared" si="0"/>
         <v>219.60784313725489</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>411.76470588235242</v>
+      </c>
+      <c r="D33">
+        <f>D32+$F$14</f>
+        <v>205.88235294117621</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>29</v>
       </c>
@@ -3532,8 +4781,16 @@
         <f t="shared" si="0"/>
         <v>227.45098039215685</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>419.60784313725435</v>
+      </c>
+      <c r="D34">
+        <f>D33+$F$14</f>
+        <v>209.80392156862717</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>30</v>
       </c>
@@ -3541,8 +4798,16 @@
         <f t="shared" si="0"/>
         <v>235.29411764705881</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>427.45098039215628</v>
+      </c>
+      <c r="D35">
+        <f>D34+$F$14</f>
+        <v>213.72549019607814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>31</v>
       </c>
@@ -3550,8 +4815,16 @@
         <f t="shared" si="0"/>
         <v>243.13725490196077</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>435.29411764705821</v>
+      </c>
+      <c r="D36">
+        <f>D35+$F$14</f>
+        <v>217.64705882352911</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>32</v>
       </c>
@@ -3559,8 +4832,16 @@
         <f t="shared" si="0"/>
         <v>250.98039215686273</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>443.13725490196015</v>
+      </c>
+      <c r="D37">
+        <f>D36+$F$14</f>
+        <v>221.56862745098007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>33</v>
       </c>
@@ -3568,8 +4849,16 @@
         <f t="shared" si="0"/>
         <v>258.8235294117647</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>450.98039215686208</v>
+      </c>
+      <c r="D38">
+        <f>D37+$F$14</f>
+        <v>225.49019607843104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>34</v>
       </c>
@@ -3577,8 +4866,16 @@
         <f t="shared" si="0"/>
         <v>266.66666666666663</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>458.82352941176401</v>
+      </c>
+      <c r="D39">
+        <f>D38+$F$14</f>
+        <v>229.41176470588201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>35</v>
       </c>
@@ -3586,8 +4883,16 @@
         <f t="shared" si="0"/>
         <v>274.50980392156862</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>466.66666666666595</v>
+      </c>
+      <c r="D40">
+        <f>D39+$F$14</f>
+        <v>233.33333333333297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>36</v>
       </c>
@@ -3595,8 +4900,16 @@
         <f t="shared" si="0"/>
         <v>282.35294117647055</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>474.50980392156788</v>
+      </c>
+      <c r="D41">
+        <f>D40+$F$14</f>
+        <v>237.25490196078394</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>37</v>
       </c>
@@ -3604,8 +4917,16 @@
         <f t="shared" si="0"/>
         <v>290.19607843137254</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>482.35294117646981</v>
+      </c>
+      <c r="D42">
+        <f>D41+$F$14</f>
+        <v>241.17647058823491</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>38</v>
       </c>
@@ -3613,8 +4934,16 @@
         <f t="shared" si="0"/>
         <v>298.03921568627447</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>490.19607843137175</v>
+      </c>
+      <c r="D43">
+        <f>D42+$F$14</f>
+        <v>245.09803921568587</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>39</v>
       </c>
@@ -3622,8 +4951,16 @@
         <f t="shared" si="0"/>
         <v>305.88235294117646</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>498.03921568627368</v>
+      </c>
+      <c r="D44">
+        <f>D43+$F$14</f>
+        <v>249.01960784313684</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>40</v>
       </c>
@@ -3631,8 +4968,16 @@
         <f t="shared" si="0"/>
         <v>313.7254901960784</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>505.88235294117561</v>
+      </c>
+      <c r="D45">
+        <f>D44+$F$14</f>
+        <v>252.94117647058781</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>41</v>
       </c>
@@ -3640,8 +4985,16 @@
         <f t="shared" si="0"/>
         <v>321.56862745098039</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>513.72549019607754</v>
+      </c>
+      <c r="D46">
+        <f>D45+$F$14</f>
+        <v>256.86274509803877</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>42</v>
       </c>
@@ -3649,8 +5002,16 @@
         <f t="shared" si="0"/>
         <v>329.41176470588232</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>521.56862745097953</v>
+      </c>
+      <c r="D47">
+        <f>D46+$F$14</f>
+        <v>260.78431372548977</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>43</v>
       </c>
@@ -3658,8 +5019,16 @@
         <f t="shared" si="0"/>
         <v>337.25490196078431</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>529.41176470588152</v>
+      </c>
+      <c r="D48">
+        <f>D47+$F$14</f>
+        <v>264.70588235294076</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>44</v>
       </c>
@@ -3667,8 +5036,16 @@
         <f t="shared" si="0"/>
         <v>345.09803921568624</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>537.25490196078351</v>
+      </c>
+      <c r="D49">
+        <f>D48+$F$14</f>
+        <v>268.62745098039176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>45</v>
       </c>
@@ -3676,8 +5053,16 @@
         <f t="shared" si="0"/>
         <v>352.94117647058823</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>545.0980392156855</v>
+      </c>
+      <c r="D50">
+        <f>D49+$F$14</f>
+        <v>272.54901960784275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>46</v>
       </c>
@@ -3685,8 +5070,16 @@
         <f t="shared" si="0"/>
         <v>360.78431372549016</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>552.94117647058749</v>
+      </c>
+      <c r="D51">
+        <f>D50+$F$14</f>
+        <v>276.47058823529375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>47</v>
       </c>
@@ -3694,8 +5087,16 @@
         <f t="shared" si="0"/>
         <v>368.62745098039215</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>560.78431372548948</v>
+      </c>
+      <c r="D52">
+        <f>D51+$F$14</f>
+        <v>280.39215686274474</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>48</v>
       </c>
@@ -3703,8 +5104,16 @@
         <f t="shared" si="0"/>
         <v>376.47058823529409</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>568.62745098039147</v>
+      </c>
+      <c r="D53">
+        <f>D52+$F$14</f>
+        <v>284.31372549019574</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>49</v>
       </c>
@@ -3712,14 +5121,30 @@
         <f t="shared" si="0"/>
         <v>384.31372549019608</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>576.47058823529346</v>
+      </c>
+      <c r="D54">
+        <f>D53+$F$14</f>
+        <v>288.23529411764673</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>50</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
         <v>392.15686274509801</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>584.31372549019545</v>
+      </c>
+      <c r="D55">
+        <f>D54+$F$14</f>
+        <v>292.15686274509773</v>
       </c>
     </row>
   </sheetData>
@@ -3733,7 +5158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D188DB2-A058-4624-9BA3-54D851F5B582}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor updates to budget calc Excel
</commit_message>
<xml_diff>
--- a/Notes/budget_calculations.xlsx
+++ b/Notes/budget_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8AED94-8E36-4B3C-9D0F-8D16DB6293D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B9113E-53DA-430A-9F68-C76CAAB193CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60A3E455-5768-4DE3-BCE2-5116B63F6CFB}"/>
   </bookViews>
@@ -4308,7 +4308,7 @@
         <v>207.84313725490196</v>
       </c>
       <c r="D7">
-        <f>D6+$F$14</f>
+        <f t="shared" ref="D7:D38" si="1">D6+$F$14</f>
         <v>103.92156862745098</v>
       </c>
     </row>
@@ -4321,11 +4321,11 @@
         <v>23.52941176470588</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C55" si="1">C7+$B$6</f>
+        <f t="shared" ref="C8:C55" si="2">C7+$B$6</f>
         <v>215.68627450980392</v>
       </c>
       <c r="D8">
-        <f>D7+$F$14</f>
+        <f t="shared" si="1"/>
         <v>107.84313725490196</v>
       </c>
     </row>
@@ -4338,11 +4338,11 @@
         <v>31.372549019607842</v>
       </c>
       <c r="C9">
+        <f t="shared" si="2"/>
+        <v>223.52941176470588</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="1"/>
-        <v>223.52941176470588</v>
-      </c>
-      <c r="D9">
-        <f>D8+$F$14</f>
         <v>111.76470588235294</v>
       </c>
       <c r="F9" t="s">
@@ -4358,11 +4358,11 @@
         <v>39.2156862745098</v>
       </c>
       <c r="C10">
+        <f t="shared" si="2"/>
+        <v>231.37254901960785</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="1"/>
-        <v>231.37254901960785</v>
-      </c>
-      <c r="D10">
-        <f>D9+$F$14</f>
         <v>115.68627450980392</v>
       </c>
       <c r="F10" t="s">
@@ -4378,11 +4378,11 @@
         <v>47.058823529411761</v>
       </c>
       <c r="C11">
+        <f t="shared" si="2"/>
+        <v>239.21568627450981</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="1"/>
-        <v>239.21568627450981</v>
-      </c>
-      <c r="D11">
-        <f>D10+$F$14</f>
         <v>119.6078431372549</v>
       </c>
       <c r="F11" t="s">
@@ -4398,11 +4398,11 @@
         <v>54.901960784313722</v>
       </c>
       <c r="C12">
+        <f t="shared" si="2"/>
+        <v>247.05882352941177</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="1"/>
-        <v>247.05882352941177</v>
-      </c>
-      <c r="D12">
-        <f>D11+$F$14</f>
         <v>123.52941176470588</v>
       </c>
       <c r="F12" t="s">
@@ -4418,11 +4418,11 @@
         <v>62.745098039215684</v>
       </c>
       <c r="C13">
+        <f t="shared" si="2"/>
+        <v>254.90196078431373</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="1"/>
-        <v>254.90196078431373</v>
-      </c>
-      <c r="D13">
-        <f>D12+$F$14</f>
         <v>127.45098039215686</v>
       </c>
       <c r="F13" t="s">
@@ -4438,11 +4438,11 @@
         <v>70.588235294117638</v>
       </c>
       <c r="C14">
+        <f t="shared" si="2"/>
+        <v>262.74509803921569</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="1"/>
-        <v>262.74509803921569</v>
-      </c>
-      <c r="D14">
-        <f>D13+$F$14</f>
         <v>131.37254901960785</v>
       </c>
       <c r="F14">
@@ -4459,11 +4459,11 @@
         <v>78.431372549019599</v>
       </c>
       <c r="C15">
+        <f t="shared" si="2"/>
+        <v>270.58823529411762</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="1"/>
-        <v>270.58823529411762</v>
-      </c>
-      <c r="D15">
-        <f>D14+$F$14</f>
         <v>135.29411764705881</v>
       </c>
     </row>
@@ -4476,11 +4476,11 @@
         <v>86.274509803921561</v>
       </c>
       <c r="C16">
+        <f t="shared" si="2"/>
+        <v>278.43137254901956</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="1"/>
-        <v>278.43137254901956</v>
-      </c>
-      <c r="D16">
-        <f>D15+$F$14</f>
         <v>139.21568627450978</v>
       </c>
     </row>
@@ -4493,11 +4493,11 @@
         <v>94.117647058823522</v>
       </c>
       <c r="C17">
+        <f t="shared" si="2"/>
+        <v>286.27450980392149</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="1"/>
-        <v>286.27450980392149</v>
-      </c>
-      <c r="D17">
-        <f>D16+$F$14</f>
         <v>143.13725490196074</v>
       </c>
     </row>
@@ -4510,11 +4510,11 @@
         <v>101.96078431372548</v>
       </c>
       <c r="C18">
+        <f t="shared" si="2"/>
+        <v>294.11764705882342</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="1"/>
-        <v>294.11764705882342</v>
-      </c>
-      <c r="D18">
-        <f>D17+$F$14</f>
         <v>147.05882352941171</v>
       </c>
     </row>
@@ -4527,11 +4527,11 @@
         <v>109.80392156862744</v>
       </c>
       <c r="C19">
+        <f t="shared" si="2"/>
+        <v>301.96078431372536</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="1"/>
-        <v>301.96078431372536</v>
-      </c>
-      <c r="D19">
-        <f>D18+$F$14</f>
         <v>150.98039215686268</v>
       </c>
     </row>
@@ -4544,11 +4544,11 @@
         <v>117.64705882352941</v>
       </c>
       <c r="C20">
+        <f t="shared" si="2"/>
+        <v>309.80392156862729</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="1"/>
-        <v>309.80392156862729</v>
-      </c>
-      <c r="D20">
-        <f>D19+$F$14</f>
         <v>154.90196078431364</v>
       </c>
     </row>
@@ -4561,11 +4561,11 @@
         <v>125.49019607843137</v>
       </c>
       <c r="C21">
+        <f t="shared" si="2"/>
+        <v>317.64705882352922</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="1"/>
-        <v>317.64705882352922</v>
-      </c>
-      <c r="D21">
-        <f>D20+$F$14</f>
         <v>158.82352941176461</v>
       </c>
     </row>
@@ -4578,11 +4578,11 @@
         <v>133.33333333333331</v>
       </c>
       <c r="C22">
+        <f t="shared" si="2"/>
+        <v>325.49019607843115</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="1"/>
-        <v>325.49019607843115</v>
-      </c>
-      <c r="D22">
-        <f>D21+$F$14</f>
         <v>162.74509803921558</v>
       </c>
     </row>
@@ -4595,11 +4595,11 @@
         <v>141.17647058823528</v>
       </c>
       <c r="C23">
+        <f t="shared" si="2"/>
+        <v>333.33333333333309</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="1"/>
-        <v>333.33333333333309</v>
-      </c>
-      <c r="D23">
-        <f>D22+$F$14</f>
         <v>166.66666666666654</v>
       </c>
     </row>
@@ -4612,11 +4612,11 @@
         <v>149.01960784313724</v>
       </c>
       <c r="C24">
+        <f t="shared" si="2"/>
+        <v>341.17647058823502</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="1"/>
-        <v>341.17647058823502</v>
-      </c>
-      <c r="D24">
-        <f>D23+$F$14</f>
         <v>170.58823529411751</v>
       </c>
     </row>
@@ -4629,11 +4629,11 @@
         <v>156.8627450980392</v>
       </c>
       <c r="C25">
+        <f t="shared" si="2"/>
+        <v>349.01960784313695</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="1"/>
-        <v>349.01960784313695</v>
-      </c>
-      <c r="D25">
-        <f>D24+$F$14</f>
         <v>174.50980392156848</v>
       </c>
     </row>
@@ -4646,11 +4646,11 @@
         <v>164.70588235294116</v>
       </c>
       <c r="C26">
+        <f t="shared" si="2"/>
+        <v>356.86274509803889</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="1"/>
-        <v>356.86274509803889</v>
-      </c>
-      <c r="D26">
-        <f>D25+$F$14</f>
         <v>178.43137254901944</v>
       </c>
     </row>
@@ -4663,11 +4663,11 @@
         <v>172.54901960784312</v>
       </c>
       <c r="C27">
+        <f t="shared" si="2"/>
+        <v>364.70588235294082</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="1"/>
-        <v>364.70588235294082</v>
-      </c>
-      <c r="D27">
-        <f>D26+$F$14</f>
         <v>182.35294117647041</v>
       </c>
     </row>
@@ -4680,11 +4680,11 @@
         <v>180.39215686274508</v>
       </c>
       <c r="C28">
+        <f t="shared" si="2"/>
+        <v>372.54901960784275</v>
+      </c>
+      <c r="D28">
         <f t="shared" si="1"/>
-        <v>372.54901960784275</v>
-      </c>
-      <c r="D28">
-        <f>D27+$F$14</f>
         <v>186.27450980392138</v>
       </c>
     </row>
@@ -4697,11 +4697,11 @@
         <v>188.23529411764704</v>
       </c>
       <c r="C29">
+        <f t="shared" si="2"/>
+        <v>380.39215686274468</v>
+      </c>
+      <c r="D29">
         <f t="shared" si="1"/>
-        <v>380.39215686274468</v>
-      </c>
-      <c r="D29">
-        <f>D28+$F$14</f>
         <v>190.19607843137234</v>
       </c>
     </row>
@@ -4714,11 +4714,11 @@
         <v>196.07843137254901</v>
       </c>
       <c r="C30">
+        <f t="shared" si="2"/>
+        <v>388.23529411764662</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="1"/>
-        <v>388.23529411764662</v>
-      </c>
-      <c r="D30">
-        <f>D29+$F$14</f>
         <v>194.11764705882331</v>
       </c>
     </row>
@@ -4731,11 +4731,11 @@
         <v>203.92156862745097</v>
       </c>
       <c r="C31">
+        <f t="shared" si="2"/>
+        <v>396.07843137254855</v>
+      </c>
+      <c r="D31">
         <f t="shared" si="1"/>
-        <v>396.07843137254855</v>
-      </c>
-      <c r="D31">
-        <f>D30+$F$14</f>
         <v>198.03921568627428</v>
       </c>
     </row>
@@ -4748,11 +4748,11 @@
         <v>211.76470588235293</v>
       </c>
       <c r="C32">
+        <f t="shared" si="2"/>
+        <v>403.92156862745048</v>
+      </c>
+      <c r="D32">
         <f t="shared" si="1"/>
-        <v>403.92156862745048</v>
-      </c>
-      <c r="D32">
-        <f>D31+$F$14</f>
         <v>201.96078431372524</v>
       </c>
     </row>
@@ -4765,11 +4765,11 @@
         <v>219.60784313725489</v>
       </c>
       <c r="C33">
+        <f t="shared" si="2"/>
+        <v>411.76470588235242</v>
+      </c>
+      <c r="D33">
         <f t="shared" si="1"/>
-        <v>411.76470588235242</v>
-      </c>
-      <c r="D33">
-        <f>D32+$F$14</f>
         <v>205.88235294117621</v>
       </c>
     </row>
@@ -4782,11 +4782,11 @@
         <v>227.45098039215685</v>
       </c>
       <c r="C34">
+        <f t="shared" si="2"/>
+        <v>419.60784313725435</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="1"/>
-        <v>419.60784313725435</v>
-      </c>
-      <c r="D34">
-        <f>D33+$F$14</f>
         <v>209.80392156862717</v>
       </c>
     </row>
@@ -4799,11 +4799,11 @@
         <v>235.29411764705881</v>
       </c>
       <c r="C35">
+        <f t="shared" si="2"/>
+        <v>427.45098039215628</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="1"/>
-        <v>427.45098039215628</v>
-      </c>
-      <c r="D35">
-        <f>D34+$F$14</f>
         <v>213.72549019607814</v>
       </c>
     </row>
@@ -4816,11 +4816,11 @@
         <v>243.13725490196077</v>
       </c>
       <c r="C36">
+        <f t="shared" si="2"/>
+        <v>435.29411764705821</v>
+      </c>
+      <c r="D36">
         <f t="shared" si="1"/>
-        <v>435.29411764705821</v>
-      </c>
-      <c r="D36">
-        <f>D35+$F$14</f>
         <v>217.64705882352911</v>
       </c>
     </row>
@@ -4833,11 +4833,11 @@
         <v>250.98039215686273</v>
       </c>
       <c r="C37">
+        <f t="shared" si="2"/>
+        <v>443.13725490196015</v>
+      </c>
+      <c r="D37">
         <f t="shared" si="1"/>
-        <v>443.13725490196015</v>
-      </c>
-      <c r="D37">
-        <f>D36+$F$14</f>
         <v>221.56862745098007</v>
       </c>
     </row>
@@ -4850,11 +4850,11 @@
         <v>258.8235294117647</v>
       </c>
       <c r="C38">
+        <f t="shared" si="2"/>
+        <v>450.98039215686208</v>
+      </c>
+      <c r="D38">
         <f t="shared" si="1"/>
-        <v>450.98039215686208</v>
-      </c>
-      <c r="D38">
-        <f>D37+$F$14</f>
         <v>225.49019607843104</v>
       </c>
     </row>
@@ -4867,11 +4867,11 @@
         <v>266.66666666666663</v>
       </c>
       <c r="C39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>458.82352941176401</v>
       </c>
       <c r="D39">
-        <f>D38+$F$14</f>
+        <f t="shared" ref="D39:D55" si="3">D38+$F$14</f>
         <v>229.41176470588201</v>
       </c>
     </row>
@@ -4884,11 +4884,11 @@
         <v>274.50980392156862</v>
       </c>
       <c r="C40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>466.66666666666595</v>
       </c>
       <c r="D40">
-        <f>D39+$F$14</f>
+        <f t="shared" si="3"/>
         <v>233.33333333333297</v>
       </c>
     </row>
@@ -4901,11 +4901,11 @@
         <v>282.35294117647055</v>
       </c>
       <c r="C41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>474.50980392156788</v>
       </c>
       <c r="D41">
-        <f>D40+$F$14</f>
+        <f t="shared" si="3"/>
         <v>237.25490196078394</v>
       </c>
     </row>
@@ -4918,11 +4918,11 @@
         <v>290.19607843137254</v>
       </c>
       <c r="C42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>482.35294117646981</v>
       </c>
       <c r="D42">
-        <f>D41+$F$14</f>
+        <f t="shared" si="3"/>
         <v>241.17647058823491</v>
       </c>
     </row>
@@ -4935,11 +4935,11 @@
         <v>298.03921568627447</v>
       </c>
       <c r="C43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>490.19607843137175</v>
       </c>
       <c r="D43">
-        <f>D42+$F$14</f>
+        <f t="shared" si="3"/>
         <v>245.09803921568587</v>
       </c>
     </row>
@@ -4952,11 +4952,11 @@
         <v>305.88235294117646</v>
       </c>
       <c r="C44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>498.03921568627368</v>
       </c>
       <c r="D44">
-        <f>D43+$F$14</f>
+        <f t="shared" si="3"/>
         <v>249.01960784313684</v>
       </c>
     </row>
@@ -4969,11 +4969,11 @@
         <v>313.7254901960784</v>
       </c>
       <c r="C45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>505.88235294117561</v>
       </c>
       <c r="D45">
-        <f>D44+$F$14</f>
+        <f t="shared" si="3"/>
         <v>252.94117647058781</v>
       </c>
     </row>
@@ -4986,11 +4986,11 @@
         <v>321.56862745098039</v>
       </c>
       <c r="C46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>513.72549019607754</v>
       </c>
       <c r="D46">
-        <f>D45+$F$14</f>
+        <f t="shared" si="3"/>
         <v>256.86274509803877</v>
       </c>
     </row>
@@ -5003,11 +5003,11 @@
         <v>329.41176470588232</v>
       </c>
       <c r="C47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>521.56862745097953</v>
       </c>
       <c r="D47">
-        <f>D46+$F$14</f>
+        <f t="shared" si="3"/>
         <v>260.78431372548977</v>
       </c>
     </row>
@@ -5020,11 +5020,11 @@
         <v>337.25490196078431</v>
       </c>
       <c r="C48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>529.41176470588152</v>
       </c>
       <c r="D48">
-        <f>D47+$F$14</f>
+        <f t="shared" si="3"/>
         <v>264.70588235294076</v>
       </c>
     </row>
@@ -5037,11 +5037,11 @@
         <v>345.09803921568624</v>
       </c>
       <c r="C49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>537.25490196078351</v>
       </c>
       <c r="D49">
-        <f>D48+$F$14</f>
+        <f t="shared" si="3"/>
         <v>268.62745098039176</v>
       </c>
     </row>
@@ -5054,11 +5054,11 @@
         <v>352.94117647058823</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>545.0980392156855</v>
       </c>
       <c r="D50">
-        <f>D49+$F$14</f>
+        <f t="shared" si="3"/>
         <v>272.54901960784275</v>
       </c>
     </row>
@@ -5071,11 +5071,11 @@
         <v>360.78431372549016</v>
       </c>
       <c r="C51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>552.94117647058749</v>
       </c>
       <c r="D51">
-        <f>D50+$F$14</f>
+        <f t="shared" si="3"/>
         <v>276.47058823529375</v>
       </c>
     </row>
@@ -5088,11 +5088,11 @@
         <v>368.62745098039215</v>
       </c>
       <c r="C52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>560.78431372548948</v>
       </c>
       <c r="D52">
-        <f>D51+$F$14</f>
+        <f t="shared" si="3"/>
         <v>280.39215686274474</v>
       </c>
     </row>
@@ -5105,11 +5105,11 @@
         <v>376.47058823529409</v>
       </c>
       <c r="C53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>568.62745098039147</v>
       </c>
       <c r="D53">
-        <f>D52+$F$14</f>
+        <f t="shared" si="3"/>
         <v>284.31372549019574</v>
       </c>
     </row>
@@ -5122,11 +5122,11 @@
         <v>384.31372549019608</v>
       </c>
       <c r="C54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>576.47058823529346</v>
       </c>
       <c r="D54">
-        <f>D53+$F$14</f>
+        <f t="shared" si="3"/>
         <v>288.23529411764673</v>
       </c>
     </row>
@@ -5139,11 +5139,11 @@
         <v>392.15686274509801</v>
       </c>
       <c r="C55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>584.31372549019545</v>
       </c>
       <c r="D55">
-        <f>D54+$F$14</f>
+        <f t="shared" si="3"/>
         <v>292.15686274509773</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating budget calulations and scenarios
</commit_message>
<xml_diff>
--- a/Notes/budget_calculations.xlsx
+++ b/Notes/budget_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_GMSE_chapters\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D174DE7-53B5-4E2F-8414-107E6C6641FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE041ED-EB3E-4531-96C2-2F72D343634A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60A3E455-5768-4DE3-BCE2-5116B63F6CFB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>time steps</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>Therefore x = 5000/1275</t>
+  </si>
+  <si>
+    <t>now I want the total to be 25000</t>
+  </si>
+  <si>
+    <t>I don't really know what I want it to start at - just not 0</t>
+  </si>
+  <si>
+    <t>25000 = 1x + 2x +30x….50x</t>
+  </si>
+  <si>
+    <t>so 25000 = 1275x</t>
+  </si>
+  <si>
+    <t>x = 20000/1275</t>
+  </si>
+  <si>
+    <t>manager budget that is constant</t>
   </si>
 </sst>
 </file>
@@ -4227,10 +4245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070648CE-F5EC-498A-AC01-A907055F7282}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4756,7 +4774,7 @@
         <v>201.96078431372524</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>28</v>
       </c>
@@ -4773,7 +4791,7 @@
         <v>205.88235294117621</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>29</v>
       </c>
@@ -4790,7 +4808,7 @@
         <v>209.80392156862717</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>30</v>
       </c>
@@ -4807,7 +4825,7 @@
         <v>213.72549019607814</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>31</v>
       </c>
@@ -4824,7 +4842,7 @@
         <v>217.64705882352911</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>32</v>
       </c>
@@ -4841,7 +4859,7 @@
         <v>221.56862745098007</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>33</v>
       </c>
@@ -4857,8 +4875,11 @@
         <f t="shared" si="1"/>
         <v>225.49019607843104</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>34</v>
       </c>
@@ -4874,8 +4895,11 @@
         <f t="shared" ref="D39:D55" si="3">D38+$F$14</f>
         <v>229.41176470588201</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>35</v>
       </c>
@@ -4891,8 +4915,11 @@
         <f t="shared" si="3"/>
         <v>233.33333333333297</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>36</v>
       </c>
@@ -4908,8 +4935,11 @@
         <f t="shared" si="3"/>
         <v>237.25490196078394</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>37</v>
       </c>
@@ -4925,8 +4955,11 @@
         <f t="shared" si="3"/>
         <v>241.17647058823491</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>38</v>
       </c>
@@ -4942,8 +4975,12 @@
         <f t="shared" si="3"/>
         <v>245.09803921568587</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H43">
+        <f>5204.1/1275</f>
+        <v>4.0816470588235294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>39</v>
       </c>
@@ -4959,8 +4996,14 @@
         <f t="shared" si="3"/>
         <v>249.01960784313684</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>40</v>
       </c>
@@ -4976,8 +5019,18 @@
         <f t="shared" si="3"/>
         <v>252.94117647058781</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <f>G44+$H$43</f>
+        <v>404.08164705882353</v>
+      </c>
+      <c r="L45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>41</v>
       </c>
@@ -4993,8 +5046,23 @@
         <f t="shared" si="3"/>
         <v>256.86274509803877</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <f>G45+$H$43</f>
+        <v>408.16329411764707</v>
+      </c>
+      <c r="I46">
+        <f>SUM(G44:G93)</f>
+        <v>25000.017647058816</v>
+      </c>
+      <c r="L46">
+        <f>25000/50</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>42</v>
       </c>
@@ -5010,8 +5078,15 @@
         <f t="shared" si="3"/>
         <v>260.78431372548977</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ref="G47:G93" si="4">G46+$H$43</f>
+        <v>412.2449411764706</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>43</v>
       </c>
@@ -5027,8 +5102,15 @@
         <f t="shared" si="3"/>
         <v>264.70588235294076</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="4"/>
+        <v>416.32658823529414</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>44</v>
       </c>
@@ -5044,8 +5126,15 @@
         <f t="shared" si="3"/>
         <v>268.62745098039176</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="4"/>
+        <v>420.40823529411767</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>45</v>
       </c>
@@ -5061,8 +5150,15 @@
         <f t="shared" si="3"/>
         <v>272.54901960784275</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>7</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="4"/>
+        <v>424.48988235294121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>46</v>
       </c>
@@ -5078,8 +5174,15 @@
         <f t="shared" si="3"/>
         <v>276.47058823529375</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="4"/>
+        <v>428.57152941176474</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>47</v>
       </c>
@@ -5095,8 +5198,15 @@
         <f t="shared" si="3"/>
         <v>280.39215686274474</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="4"/>
+        <v>432.65317647058828</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>48</v>
       </c>
@@ -5112,8 +5222,15 @@
         <f t="shared" si="3"/>
         <v>284.31372549019574</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="4"/>
+        <v>436.73482352941181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>49</v>
       </c>
@@ -5129,8 +5246,15 @@
         <f t="shared" si="3"/>
         <v>288.23529411764673</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>11</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="4"/>
+        <v>440.81647058823535</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>50</v>
       </c>
@@ -5145,6 +5269,355 @@
       <c r="D55">
         <f t="shared" si="3"/>
         <v>292.15686274509773</v>
+      </c>
+      <c r="F55">
+        <v>12</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="4"/>
+        <v>444.89811764705888</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <v>13</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="4"/>
+        <v>448.97976470588242</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <v>14</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="4"/>
+        <v>453.06141176470595</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>15</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="4"/>
+        <v>457.14305882352949</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>16</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="4"/>
+        <v>461.22470588235302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>17</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="4"/>
+        <v>465.30635294117656</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <v>18</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="4"/>
+        <v>469.38800000000009</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>19</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="4"/>
+        <v>473.46964705882363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>20</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="4"/>
+        <v>477.55129411764716</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>21</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="4"/>
+        <v>481.63294117647069</v>
+      </c>
+    </row>
+    <row r="65" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>22</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="4"/>
+        <v>485.71458823529423</v>
+      </c>
+    </row>
+    <row r="66" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>23</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="4"/>
+        <v>489.79623529411776</v>
+      </c>
+    </row>
+    <row r="67" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>24</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="4"/>
+        <v>493.8778823529413</v>
+      </c>
+    </row>
+    <row r="68" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>25</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="4"/>
+        <v>497.95952941176483</v>
+      </c>
+    </row>
+    <row r="69" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>26</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>502.04117647058837</v>
+      </c>
+    </row>
+    <row r="70" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>27</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>506.1228235294119</v>
+      </c>
+    </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>28</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>510.20447058823544</v>
+      </c>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>29</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>514.28611764705897</v>
+      </c>
+    </row>
+    <row r="73" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>30</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>518.36776470588245</v>
+      </c>
+    </row>
+    <row r="74" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>31</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>522.44941176470593</v>
+      </c>
+    </row>
+    <row r="75" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>32</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>526.53105882352941</v>
+      </c>
+    </row>
+    <row r="76" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>33</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>530.61270588235288</v>
+      </c>
+    </row>
+    <row r="77" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>34</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>534.69435294117636</v>
+      </c>
+    </row>
+    <row r="78" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>35</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>538.77599999999984</v>
+      </c>
+    </row>
+    <row r="79" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>36</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>542.85764705882332</v>
+      </c>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>37</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>546.9392941176468</v>
+      </c>
+    </row>
+    <row r="81" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>38</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="4"/>
+        <v>551.02094117647027</v>
+      </c>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>39</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="4"/>
+        <v>555.10258823529375</v>
+      </c>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>40</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="4"/>
+        <v>559.18423529411723</v>
+      </c>
+    </row>
+    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>41</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="4"/>
+        <v>563.26588235294071</v>
+      </c>
+    </row>
+    <row r="85" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>42</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="4"/>
+        <v>567.34752941176419</v>
+      </c>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>43</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="4"/>
+        <v>571.42917647058766</v>
+      </c>
+    </row>
+    <row r="87" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <v>44</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="4"/>
+        <v>575.51082352941114</v>
+      </c>
+    </row>
+    <row r="88" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <v>45</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="4"/>
+        <v>579.59247058823462</v>
+      </c>
+    </row>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>46</v>
+      </c>
+      <c r="G89">
+        <f t="shared" si="4"/>
+        <v>583.6741176470581</v>
+      </c>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>47</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="4"/>
+        <v>587.75576470588157</v>
+      </c>
+    </row>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>48</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="4"/>
+        <v>591.83741176470505</v>
+      </c>
+    </row>
+    <row r="92" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>49</v>
+      </c>
+      <c r="G92">
+        <f t="shared" si="4"/>
+        <v>595.91905882352853</v>
+      </c>
+    </row>
+    <row r="93" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>50</v>
+      </c>
+      <c r="G93">
+        <f t="shared" si="4"/>
+        <v>600.00070588235201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>